<commit_message>
Added error control. Tested interpolation code. Added Boresight Gain for Helical Antennas Added Gain over all angles for Helical Antennas
</commit_message>
<xml_diff>
--- a/data/Antenna/BoresightGainDataHelicalAntennas.xlsx
+++ b/data/Antenna/BoresightGainDataHelicalAntennas.xlsx
@@ -13,15 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="3" uniqueCount="3">
   <si>
     <t>Frequency (Hz)</t>
   </si>
   <si>
-    <t>Boresight Gain (dBi)</t>
-  </si>
-  <si>
-    <t>S21 (dB)</t>
+    <t>Gain (dBi)</t>
   </si>
   <si>
     <t>Return Loss (dB)</t>
@@ -70,16 +67,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D202"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.36328125" customWidth="true"/>
-    <col min="2" max="2" width="17.36328125" customWidth="true"/>
-    <col min="3" max="3" width="12.08984375" customWidth="true"/>
-    <col min="4" max="4" width="14.453125" customWidth="true"/>
+    <col min="2" max="2" width="14.453125" customWidth="true"/>
+    <col min="3" max="3" width="14.453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -92,22 +88,16 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
         <v>1000000000</v>
       </c>
       <c r="B2" s="0">
-        <v>-10.448746913167511</v>
+        <v>-11.008595878716942</v>
       </c>
       <c r="C2" s="0">
-        <v>-57.124579391074668</v>
-      </c>
-      <c r="D2" s="0">
-        <v>-1.0971431239715488</v>
+        <v>-1.0970920240398798</v>
       </c>
     </row>
     <row r="3">
@@ -115,13 +105,10 @@
         <v>1015000000</v>
       </c>
       <c r="B3" s="0">
-        <v>-11.072626313596253</v>
+        <v>-11.212376549828384</v>
       </c>
       <c r="C3" s="0">
-        <v>-58.501659036916777</v>
-      </c>
-      <c r="D3" s="0">
-        <v>-0.94350545247216067</v>
+        <v>-0.92781794077833435</v>
       </c>
     </row>
     <row r="4">
@@ -129,13 +116,10 @@
         <v>1030000000</v>
       </c>
       <c r="B4" s="0">
-        <v>-13.051443726934824</v>
+        <v>-13.624513360781382</v>
       </c>
       <c r="C4" s="0">
-        <v>-62.586717512712738</v>
-      </c>
-      <c r="D4" s="0">
-        <v>-1.4005231091657904</v>
+        <v>-1.4033348642067847</v>
       </c>
     </row>
     <row r="5">
@@ -143,13 +127,10 @@
         <v>1045000000</v>
       </c>
       <c r="B5" s="0">
-        <v>-12.278769524355699</v>
+        <v>-12.282942531738357</v>
       </c>
       <c r="C5" s="0">
-        <v>-61.166950422392496</v>
-      </c>
-      <c r="D5" s="0">
-        <v>-3.014192382680652</v>
+        <v>-3.0006418771069612</v>
       </c>
     </row>
     <row r="6">
@@ -157,13 +138,10 @@
         <v>1060000000</v>
       </c>
       <c r="B6" s="0">
-        <v>-10.112285853045588</v>
+        <v>-10.380894066791196</v>
       </c>
       <c r="C6" s="0">
-        <v>-56.957774576126226</v>
-      </c>
-      <c r="D6" s="0">
-        <v>-7.2100345419382954</v>
+        <v>-7.1429221869842312</v>
       </c>
     </row>
     <row r="7">
@@ -171,13 +149,10 @@
         <v>1075000000</v>
       </c>
       <c r="B7" s="0">
-        <v>-11.344261895849176</v>
+        <v>-12.003576974071461</v>
       </c>
       <c r="C7" s="0">
-        <v>-59.543778641470482</v>
-      </c>
-      <c r="D7" s="0">
-        <v>-3.4768888243343943</v>
+        <v>-3.4666450300920997</v>
       </c>
     </row>
     <row r="8">
@@ -185,13 +160,10 @@
         <v>1090000000</v>
       </c>
       <c r="B8" s="0">
-        <v>-15.139587839057004</v>
+        <v>-13.854136390931313</v>
       </c>
       <c r="C8" s="0">
-        <v>-67.254791201666123</v>
-      </c>
-      <c r="D8" s="0">
-        <v>-1.6369330369617783</v>
+        <v>-1.6487386151290653</v>
       </c>
     </row>
     <row r="9">
@@ -199,13 +171,10 @@
         <v>1105000000</v>
       </c>
       <c r="B9" s="0">
-        <v>-14.774060809953735</v>
+        <v>-14.032527606266502</v>
       </c>
       <c r="C9" s="0">
-        <v>-66.642452745069704</v>
-      </c>
-      <c r="D9" s="0">
-        <v>-1.5470363368482623</v>
+        <v>-1.5331971239618489</v>
       </c>
     </row>
     <row r="10">
@@ -213,13 +182,10 @@
         <v>1120000000</v>
       </c>
       <c r="B10" s="0">
-        <v>-11.043580968167937</v>
+        <v>-11.513989302604067</v>
       </c>
       <c r="C10" s="0">
-        <v>-59.298607954479152</v>
-      </c>
-      <c r="D10" s="0">
-        <v>-2.4513549768381244</v>
+        <v>-2.4449845776686758</v>
       </c>
     </row>
     <row r="11">
@@ -227,13 +193,10 @@
         <v>1135000000</v>
       </c>
       <c r="B11" s="0">
-        <v>-6.9742076570848752</v>
+        <v>-7.5844834681066899</v>
       </c>
       <c r="C11" s="0">
-        <v>-51.275418109492222</v>
-      </c>
-      <c r="D11" s="0">
-        <v>-6.0249731296830937</v>
+        <v>-5.95208222992638</v>
       </c>
     </row>
     <row r="12">
@@ -241,13 +204,10 @@
         <v>1150000000</v>
       </c>
       <c r="B12" s="0">
-        <v>-6.6891997741569398</v>
+        <v>-6.7179094830126544</v>
       </c>
       <c r="C12" s="0">
-        <v>-50.819441920125755</v>
-      </c>
-      <c r="D12" s="0">
-        <v>-6.0132786359754276</v>
+        <v>-6.0015980979064674</v>
       </c>
     </row>
     <row r="13">
@@ -255,13 +215,10 @@
         <v>1165000000</v>
       </c>
       <c r="B13" s="0">
-        <v>-9.6550934451138062</v>
+        <v>-10.122883473242723</v>
       </c>
       <c r="C13" s="0">
-        <v>-56.863790962208007</v>
-      </c>
-      <c r="D13" s="0">
-        <v>-2.5982216675234397</v>
+        <v>-2.6004560500297504</v>
       </c>
     </row>
     <row r="14">
@@ -269,13 +226,10 @@
         <v>1180000000</v>
       </c>
       <c r="B14" s="0">
-        <v>-13.164925530125689</v>
+        <v>-14.251734199515067</v>
       </c>
       <c r="C14" s="0">
-        <v>-63.994576771113529</v>
-      </c>
-      <c r="D14" s="0">
-        <v>-1.6017639456322579</v>
+        <v>-1.6164343928853335</v>
       </c>
     </row>
     <row r="15">
@@ -283,13 +237,10 @@
         <v>1195000000</v>
       </c>
       <c r="B15" s="0">
-        <v>-11.518229279494555</v>
+        <v>-11.499140099641462</v>
       </c>
       <c r="C15" s="0">
-        <v>-60.810902229411887</v>
-      </c>
-      <c r="D15" s="0">
-        <v>-1.4424431036335443</v>
+        <v>-1.4297034701125957</v>
       </c>
     </row>
     <row r="16">
@@ -297,13 +248,10 @@
         <v>1210000000</v>
       </c>
       <c r="B16" s="0">
-        <v>-14.837225186080811</v>
+        <v>-13.524845342971187</v>
       </c>
       <c r="C16" s="0">
-        <v>-67.557243343230269</v>
-      </c>
-      <c r="D16" s="0">
-        <v>-2.1092818430118805</v>
+        <v>-2.1246623258036084</v>
       </c>
     </row>
     <row r="17">
@@ -311,13 +259,10 @@
         <v>1225000000</v>
       </c>
       <c r="B17" s="0">
-        <v>-9.1469311433977616</v>
+        <v>-9.2349756272518597</v>
       </c>
       <c r="C17" s="0">
-        <v>-56.283669625546189</v>
-      </c>
-      <c r="D17" s="0">
-        <v>-4.7809786403450492</v>
+        <v>-4.7257496839705873</v>
       </c>
     </row>
     <row r="18">
@@ -325,13 +270,10 @@
         <v>1240000000</v>
       </c>
       <c r="B18" s="0">
-        <v>-7.7199348433593187</v>
+        <v>-7.2071612294493832</v>
       </c>
       <c r="C18" s="0">
-        <v>-53.535388954702981</v>
-      </c>
-      <c r="D18" s="0">
-        <v>-6.6664675763683023</v>
+        <v>-6.635836231408339</v>
       </c>
     </row>
     <row r="19">
@@ -339,13 +281,10 @@
         <v>1255000000</v>
       </c>
       <c r="B19" s="0">
-        <v>-14.501301367710692</v>
+        <v>-14.204377913231976</v>
       </c>
       <c r="C19" s="0">
-        <v>-67.202562816502166</v>
-      </c>
-      <c r="D19" s="0">
-        <v>-3.0402199098492586</v>
+        <v>-3.023775450266518</v>
       </c>
     </row>
     <row r="20">
@@ -353,13 +292,10 @@
         <v>1270000000</v>
       </c>
       <c r="B20" s="0">
-        <v>-5.1219936143902949</v>
+        <v>-5.2149070864246845</v>
       </c>
       <c r="C20" s="0">
-        <v>-48.547147212639373</v>
-      </c>
-      <c r="D20" s="0">
-        <v>-1.7876039814971185</v>
+        <v>-1.7930542724802296</v>
       </c>
     </row>
     <row r="21">
@@ -367,13 +303,10 @@
         <v>1285000000</v>
       </c>
       <c r="B21" s="0">
-        <v>-3.5717892472357633</v>
+        <v>-3.5412986059001526</v>
       </c>
       <c r="C21" s="0">
-        <v>-45.548726612557431</v>
-      </c>
-      <c r="D21" s="0">
-        <v>-1.5619714577505048</v>
+        <v>-1.5870625689972637</v>
       </c>
     </row>
     <row r="22">
@@ -381,13 +314,10 @@
         <v>1300000000</v>
       </c>
       <c r="B22" s="0">
-        <v>-4.607000839043323</v>
+        <v>-4.5600949160973734</v>
       </c>
       <c r="C22" s="0">
-        <v>-47.719954288963024</v>
-      </c>
-      <c r="D22" s="0">
-        <v>-2.0399162074411499</v>
+        <v>-2.0511938016921492</v>
       </c>
     </row>
     <row r="23">
@@ -395,13 +325,10 @@
         <v>1315000000</v>
       </c>
       <c r="B23" s="0">
-        <v>-9.5910275359004729</v>
+        <v>-9.9340135225116093</v>
       </c>
       <c r="C23" s="0">
-        <v>-57.787655693056124</v>
-      </c>
-      <c r="D23" s="0">
-        <v>-4.4457461251463108</v>
+        <v>-4.413687278404975</v>
       </c>
     </row>
     <row r="24">
@@ -409,13 +336,10 @@
         <v>1330000000</v>
       </c>
       <c r="B24" s="0">
-        <v>-4.8160908707453522</v>
+        <v>-5.0403644796930074</v>
       </c>
       <c r="C24" s="0">
-        <v>-48.336300125572066</v>
-      </c>
-      <c r="D24" s="0">
-        <v>-8.8839013031397229</v>
+        <v>-8.811534794344178</v>
       </c>
     </row>
     <row r="25">
@@ -423,13 +347,10 @@
         <v>1345000000</v>
       </c>
       <c r="B25" s="0">
-        <v>-3.2266845043786567</v>
+        <v>-3.3431817179841801</v>
       </c>
       <c r="C25" s="0">
-        <v>-45.254900260265494</v>
-      </c>
-      <c r="D25" s="0">
-        <v>-5.0137625305361722</v>
+        <v>-5.0117861003409274</v>
       </c>
     </row>
     <row r="26">
@@ -437,13 +358,10 @@
         <v>1360000000</v>
       </c>
       <c r="B26" s="0">
-        <v>-5.4786483637529599</v>
+        <v>-5.6979780960830482</v>
       </c>
       <c r="C26" s="0">
-        <v>-49.855160459649916</v>
-      </c>
-      <c r="D26" s="0">
-        <v>-2.4574030696398284</v>
+        <v>-2.4661176790737289</v>
       </c>
     </row>
     <row r="27">
@@ -451,13 +369,10 @@
         <v>1375000000</v>
       </c>
       <c r="B27" s="0">
-        <v>-9.2922051183064767</v>
+        <v>-8.4043384892886905</v>
       </c>
       <c r="C27" s="0">
-        <v>-57.577549764678224</v>
-      </c>
-      <c r="D27" s="0">
-        <v>-1.7390625315013124</v>
+        <v>-1.7637418497250781</v>
       </c>
     </row>
     <row r="28">
@@ -465,13 +380,10 @@
         <v>1390000000</v>
       </c>
       <c r="B28" s="0">
-        <v>-10.847597156850288</v>
+        <v>-10.378840607996974</v>
       </c>
       <c r="C28" s="0">
-        <v>-60.782575883522121</v>
-      </c>
-      <c r="D28" s="0">
-        <v>-2.2275589277848851</v>
+        <v>-2.234828059685726</v>
       </c>
     </row>
     <row r="29">
@@ -479,13 +391,10 @@
         <v>1405000000</v>
       </c>
       <c r="B29" s="0">
-        <v>-4.5658418226819606</v>
+        <v>-4.5895535803952896</v>
       </c>
       <c r="C29" s="0">
-        <v>-48.312295694925538</v>
-      </c>
-      <c r="D29" s="0">
-        <v>-5.0136852885232734</v>
+        <v>-4.9922777285613469</v>
       </c>
     </row>
     <row r="30">
@@ -493,13 +402,10 @@
         <v>1420000000</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.55926032352382293</v>
+        <v>-0.45493597932570395</v>
       </c>
       <c r="C30" s="0">
-        <v>-40.391373099448415</v>
-      </c>
-      <c r="D30" s="0">
-        <v>-12.626794241119285</v>
+        <v>-12.586343054293172</v>
       </c>
     </row>
     <row r="31">
@@ -507,13 +413,10 @@
         <v>1435000000</v>
       </c>
       <c r="B31" s="0">
-        <v>-0.60400221340527338</v>
+        <v>-0.65562548485315375</v>
       </c>
       <c r="C31" s="0">
-        <v>-40.572128012950408</v>
-      </c>
-      <c r="D31" s="0">
-        <v>-6.6953037442810199</v>
+        <v>-6.6026753373682983</v>
       </c>
     </row>
     <row r="32">
@@ -521,13 +424,10 @@
         <v>1450000000</v>
       </c>
       <c r="B32" s="0">
-        <v>-7.6631409727385282</v>
+        <v>-7.3877761053244093</v>
       </c>
       <c r="C32" s="0">
-        <v>-54.780727554916197</v>
-      </c>
-      <c r="D32" s="0">
-        <v>-3.7168467777294389</v>
+        <v>-3.7394679311136816</v>
       </c>
     </row>
     <row r="33">
@@ -535,13 +435,10 @@
         <v>1465000000</v>
       </c>
       <c r="B33" s="0">
-        <v>-0.161896495145605</v>
+        <v>-0.20879068888451968</v>
       </c>
       <c r="C33" s="0">
-        <v>-39.867631048833417</v>
-      </c>
-      <c r="D33" s="0">
-        <v>-2.7796731112121957</v>
+        <v>-2.7688447934912848</v>
       </c>
     </row>
     <row r="34">
@@ -549,13 +446,10 @@
         <v>1480000000</v>
       </c>
       <c r="B34" s="0">
-        <v>2.6208904322653375</v>
+        <v>2.5895608740772929</v>
       </c>
       <c r="C34" s="0">
-        <v>-34.390539008108114</v>
-      </c>
-      <c r="D34" s="0">
-        <v>-2.9769967533878243</v>
+        <v>-2.9903441689284103</v>
       </c>
     </row>
     <row r="35">
@@ -563,13 +457,10 @@
         <v>1495000000</v>
       </c>
       <c r="B35" s="0">
-        <v>3.1433261454617671</v>
+        <v>3.1623553268734348</v>
       </c>
       <c r="C35" s="0">
-        <v>-33.43325712702508</v>
-      </c>
-      <c r="D35" s="0">
-        <v>-4.7825501911535051</v>
+        <v>-4.7642096465189203</v>
       </c>
     </row>
     <row r="36">
@@ -577,13 +468,10 @@
         <v>1510000000</v>
       </c>
       <c r="B36" s="0">
-        <v>1.6528092538449748</v>
+        <v>1.6864356078610534</v>
       </c>
       <c r="C36" s="0">
-        <v>-36.50100600291308</v>
-      </c>
-      <c r="D36" s="0">
-        <v>-11.690970189756044</v>
+        <v>-11.63819023719849</v>
       </c>
     </row>
     <row r="37">
@@ -591,13 +479,10 @@
         <v>1525000000</v>
       </c>
       <c r="B37" s="0">
-        <v>-1.8496140926505866</v>
+        <v>-1.8570141494956118</v>
       </c>
       <c r="C37" s="0">
-        <v>-43.591710623696905</v>
-      </c>
-      <c r="D37" s="0">
-        <v>-8.8774515828170237</v>
+        <v>-8.8143869125391046</v>
       </c>
     </row>
     <row r="38">
@@ -605,13 +490,10 @@
         <v>1540000000</v>
       </c>
       <c r="B38" s="0">
-        <v>-2.6478786435849138</v>
+        <v>-2.6099357453783263</v>
       </c>
       <c r="C38" s="0">
-        <v>-45.27325726863873</v>
-      </c>
-      <c r="D38" s="0">
-        <v>-3.8779461882217685</v>
+        <v>-3.8448047535527201</v>
       </c>
     </row>
     <row r="39">
@@ -619,13 +501,10 @@
         <v>1555000000</v>
       </c>
       <c r="B39" s="0">
-        <v>-5.082370672809958</v>
+        <v>-5.6039777193241171</v>
       </c>
       <c r="C39" s="0">
-        <v>-50.226434777616682</v>
-      </c>
-      <c r="D39" s="0">
-        <v>-2.307278345338772</v>
+        <v>-2.3011104798069599</v>
       </c>
     </row>
     <row r="40">
@@ -633,13 +512,10 @@
         <v>1570000000</v>
       </c>
       <c r="B40" s="0">
-        <v>-1.4310441535735201</v>
+        <v>-1.3616960580081674</v>
       </c>
       <c r="C40" s="0">
-        <v>-43.007166920071363</v>
-      </c>
-      <c r="D40" s="0">
-        <v>-2.8854960297998105</v>
+        <v>-2.8726155806048173</v>
       </c>
     </row>
     <row r="41">
@@ -647,13 +523,10 @@
         <v>1585000000</v>
       </c>
       <c r="B41" s="0">
-        <v>-2.1127841902690854</v>
+        <v>-2.2311625533557624</v>
       </c>
       <c r="C41" s="0">
-        <v>-44.453239276353223</v>
-      </c>
-      <c r="D41" s="0">
-        <v>-6.6867184504402468</v>
+        <v>-6.6511133936663471</v>
       </c>
     </row>
     <row r="42">
@@ -661,13 +534,10 @@
         <v>1600000000</v>
       </c>
       <c r="B42" s="0">
-        <v>4.1224870513151544</v>
+        <v>4.1442033938642524</v>
       </c>
       <c r="C42" s="0">
-        <v>-32.06451111522783</v>
-      </c>
-      <c r="D42" s="0">
-        <v>-18.108483754344576</v>
+        <v>-18.333056121809001</v>
       </c>
     </row>
     <row r="43">
@@ -675,13 +545,10 @@
         <v>1615000000</v>
       </c>
       <c r="B43" s="0">
-        <v>5.5427641563935417</v>
+        <v>5.5632213053806137</v>
       </c>
       <c r="C43" s="0">
-        <v>-29.30500778529499</v>
-      </c>
-      <c r="D43" s="0">
-        <v>-10.873989675238128</v>
+        <v>-10.856620541558314</v>
       </c>
     </row>
     <row r="44">
@@ -689,13 +556,10 @@
         <v>1630000000</v>
       </c>
       <c r="B44" s="0">
-        <v>5.2474177616623621</v>
+        <v>5.2802639651755303</v>
       </c>
       <c r="C44" s="0">
-        <v>-29.976002129494077</v>
-      </c>
-      <c r="D44" s="0">
-        <v>-6.6406568412854261</v>
+        <v>-6.5749430779056741</v>
       </c>
     </row>
     <row r="45">
@@ -703,13 +567,10 @@
         <v>1645000000</v>
       </c>
       <c r="B45" s="0">
-        <v>2.8451828449264696</v>
+        <v>2.8728622246342148</v>
       </c>
       <c r="C45" s="0">
-        <v>-34.860037920606565</v>
-      </c>
-      <c r="D45" s="0">
-        <v>-4.1850058959813694</v>
+        <v>-4.1824394077412403</v>
       </c>
     </row>
     <row r="46">
@@ -717,13 +578,10 @@
         <v>1660000000</v>
       </c>
       <c r="B46" s="0">
-        <v>-6.4817424746201588</v>
+        <v>-6.6115982909478284</v>
       </c>
       <c r="C46" s="0">
-        <v>-53.592732274781063</v>
-      </c>
-      <c r="D46" s="0">
-        <v>-6.6886475470352593</v>
+        <v>-6.5902719177240696</v>
       </c>
     </row>
     <row r="47">
@@ -731,13 +589,10 @@
         <v>1675000000</v>
       </c>
       <c r="B47" s="0">
-        <v>0.66366966983273556</v>
+        <v>0.63127824423520451</v>
       </c>
       <c r="C47" s="0">
-        <v>-39.380042452531455</v>
-      </c>
-      <c r="D47" s="0">
-        <v>-7.9627526006414495</v>
+        <v>-7.8904370846412828</v>
       </c>
     </row>
     <row r="48">
@@ -745,13 +600,10 @@
         <v>1690000000</v>
       </c>
       <c r="B48" s="0">
-        <v>6.1595217204652393</v>
+        <v>6.0986540906708022</v>
       </c>
       <c r="C48" s="0">
-        <v>-28.465776216082631</v>
-      </c>
-      <c r="D48" s="0">
-        <v>-5.8090271768925721</v>
+        <v>-5.8180140783211876</v>
       </c>
     </row>
     <row r="49">
@@ -759,13 +611,10 @@
         <v>1705000000</v>
       </c>
       <c r="B49" s="0">
-        <v>7.8107784896569949</v>
+        <v>7.7795797279392218</v>
       </c>
       <c r="C49" s="0">
-        <v>-25.240016251995986</v>
-      </c>
-      <c r="D49" s="0">
-        <v>-6.4413155901959493</v>
+        <v>-6.3618816456173004</v>
       </c>
     </row>
     <row r="50">
@@ -773,13 +622,10 @@
         <v>1720000000</v>
       </c>
       <c r="B50" s="0">
-        <v>8.2197428355300701</v>
+        <v>8.2153548852782912</v>
       </c>
       <c r="C50" s="0">
-        <v>-24.498168831830483</v>
-      </c>
-      <c r="D50" s="0">
-        <v>-7.345273239543233</v>
+        <v>-7.3653202164246103</v>
       </c>
     </row>
     <row r="51">
@@ -787,13 +633,10 @@
         <v>1735000000</v>
       </c>
       <c r="B51" s="0">
-        <v>8.5460340092557523</v>
+        <v>8.526544400649108</v>
       </c>
       <c r="C51" s="0">
-        <v>-23.921007128765993</v>
-      </c>
-      <c r="D51" s="0">
-        <v>-8.1014359825370228</v>
+        <v>-8.1110580027633485</v>
       </c>
     </row>
     <row r="52">
@@ -801,13 +644,10 @@
         <v>1750000000</v>
       </c>
       <c r="B52" s="0">
-        <v>8.8178184713516821</v>
+        <v>8.7654255181501153</v>
       </c>
       <c r="C52" s="0">
-        <v>-23.452209595762163</v>
-      </c>
-      <c r="D52" s="0">
-        <v>-8.1198410869910891</v>
+        <v>-8.0201877608241237</v>
       </c>
     </row>
     <row r="53">
@@ -815,13 +655,10 @@
         <v>1765000000</v>
       </c>
       <c r="B53" s="0">
-        <v>8.9890439851912767</v>
+        <v>8.915214666093668</v>
       </c>
       <c r="C53" s="0">
-        <v>-23.183891788833918</v>
-      </c>
-      <c r="D53" s="0">
-        <v>-8.2005536975642848</v>
+        <v>-8.2526797911637999</v>
       </c>
     </row>
     <row r="54">
@@ -829,13 +666,10 @@
         <v>1780000000</v>
       </c>
       <c r="B54" s="0">
-        <v>9.1034431306169399</v>
+        <v>9.019941973187553</v>
       </c>
       <c r="C54" s="0">
-        <v>-23.028599349683642</v>
-      </c>
-      <c r="D54" s="0">
-        <v>-8.9330948406324477</v>
+        <v>-8.8981918325180924</v>
       </c>
     </row>
     <row r="55">
@@ -843,13 +677,10 @@
         <v>1795000000</v>
       </c>
       <c r="B55" s="0">
-        <v>9.1628038484714747</v>
+        <v>9.0622477678211606</v>
       </c>
       <c r="C55" s="0">
-        <v>-22.982766926083453</v>
-      </c>
-      <c r="D55" s="0">
-        <v>-8.9524625657599213</v>
+        <v>-8.8841753324517079</v>
       </c>
     </row>
     <row r="56">
@@ -857,13 +688,10 @@
         <v>1810000000</v>
       </c>
       <c r="B56" s="0">
-        <v>9.2033875393861635</v>
+        <v>9.0752946642774326</v>
       </c>
       <c r="C56" s="0">
-        <v>-22.973881983351006</v>
-      </c>
-      <c r="D56" s="0">
-        <v>-8.9698468735191135</v>
+        <v>-9.0106314226369619</v>
       </c>
     </row>
     <row r="57">
@@ -871,13 +699,10 @@
         <v>1825000000</v>
       </c>
       <c r="B57" s="0">
-        <v>9.2454060990922002</v>
+        <v>9.1210064245754658</v>
       </c>
       <c r="C57" s="0">
-        <v>-22.961530742405117</v>
-      </c>
-      <c r="D57" s="0">
-        <v>-9.8483076370959708</v>
+        <v>-9.7625181156857117</v>
       </c>
     </row>
     <row r="58">
@@ -885,13 +710,10 @@
         <v>1840000000</v>
       </c>
       <c r="B58" s="0">
-        <v>9.2302202731336518</v>
+        <v>9.1541600584728915</v>
       </c>
       <c r="C58" s="0">
-        <v>-23.063001478663065</v>
-      </c>
-      <c r="D58" s="0">
-        <v>-10.163597189408373</v>
+        <v>-10.032728438039873</v>
       </c>
     </row>
     <row r="59">
@@ -899,13 +721,10 @@
         <v>1855000000</v>
       </c>
       <c r="B59" s="0">
-        <v>9.2907165045076567</v>
+        <v>9.2875620896339406</v>
       </c>
       <c r="C59" s="0">
-        <v>-23.012530834745625</v>
-      </c>
-      <c r="D59" s="0">
-        <v>-10.256462698135262</v>
+        <v>-10.251704177647202</v>
       </c>
     </row>
     <row r="60">
@@ -913,13 +732,10 @@
         <v>1870000000</v>
       </c>
       <c r="B60" s="0">
-        <v>9.3727556012031865</v>
+        <v>9.4188618440108574</v>
       </c>
       <c r="C60" s="0">
-        <v>-22.918406493063248</v>
-      </c>
-      <c r="D60" s="0">
-        <v>-11.026020746800569</v>
+        <v>-10.898513809673878</v>
       </c>
     </row>
     <row r="61">
@@ -927,13 +743,10 @@
         <v>1885000000</v>
       </c>
       <c r="B61" s="0">
-        <v>9.5410581602824607</v>
+        <v>9.5864390554941288</v>
       </c>
       <c r="C61" s="0">
-        <v>-22.651196335010951</v>
-      </c>
-      <c r="D61" s="0">
-        <v>-11.659926548714466</v>
+        <v>-11.380567669493988</v>
       </c>
     </row>
     <row r="62">
@@ -941,13 +754,10 @@
         <v>1900000000</v>
       </c>
       <c r="B62" s="0">
-        <v>9.7098180589396392</v>
+        <v>9.7327320509359101</v>
       </c>
       <c r="C62" s="0">
-        <v>-22.382521465916952</v>
-      </c>
-      <c r="D62" s="0">
-        <v>-12.001287077522612</v>
+        <v>-11.776129741639942</v>
       </c>
     </row>
     <row r="63">
@@ -955,13 +765,10 @@
         <v>1915000000</v>
       </c>
       <c r="B63" s="0">
-        <v>9.8664206990698489</v>
+        <v>9.8779138668531523</v>
       </c>
       <c r="C63" s="0">
-        <v>-22.137619732692777</v>
-      </c>
-      <c r="D63" s="0">
-        <v>-12.392556738436976</v>
+        <v>-11.997812293628893</v>
       </c>
     </row>
     <row r="64">
@@ -969,13 +776,10 @@
         <v>1930000000</v>
       </c>
       <c r="B64" s="0">
-        <v>10.059102766995771</v>
+        <v>10.047479292360386</v>
       </c>
       <c r="C64" s="0">
-        <v>-21.820026210903578</v>
-      </c>
-      <c r="D64" s="0">
-        <v>-13.456107269508069</v>
+        <v>-12.725735916509848</v>
       </c>
     </row>
     <row r="65">
@@ -983,13 +787,10 @@
         <v>1945000000</v>
       </c>
       <c r="B65" s="0">
-        <v>10.220231109554092</v>
+        <v>10.193101595377119</v>
       </c>
       <c r="C65" s="0">
-        <v>-21.565015458865986</v>
-      </c>
-      <c r="D65" s="0">
-        <v>-14.124472949047359</v>
+        <v>-13.382773996977944</v>
       </c>
     </row>
     <row r="66">
@@ -997,13 +798,10 @@
         <v>1960000000</v>
       </c>
       <c r="B66" s="0">
-        <v>10.377177618738394</v>
+        <v>10.336045036416568</v>
       </c>
       <c r="C66" s="0">
-        <v>-21.317851754392372</v>
-      </c>
-      <c r="D66" s="0">
-        <v>-14.130936950684498</v>
+        <v>-13.541481018870138</v>
       </c>
     </row>
     <row r="67">
@@ -1011,13 +809,10 @@
         <v>1975000000</v>
       </c>
       <c r="B67" s="0">
-        <v>10.533836461800274</v>
+        <v>10.493191263634507</v>
       </c>
       <c r="C67" s="0">
-        <v>-21.070754640388678</v>
-      </c>
-      <c r="D67" s="0">
-        <v>-15.079367227495572</v>
+        <v>-14.321213196438066</v>
       </c>
     </row>
     <row r="68">
@@ -1025,13 +820,10 @@
         <v>1990000000</v>
       </c>
       <c r="B68" s="0">
-        <v>10.69307862845881</v>
+        <v>10.662668687227427</v>
       </c>
       <c r="C68" s="0">
-        <v>-20.81798983601616</v>
-      </c>
-      <c r="D68" s="0">
-        <v>-15.822972802409115</v>
+        <v>-15.354978324320825</v>
       </c>
     </row>
     <row r="69">
@@ -1039,13 +831,10 @@
         <v>2005000000</v>
       </c>
       <c r="B69" s="0">
-        <v>10.925676422670918</v>
+        <v>10.919095763389709</v>
       </c>
       <c r="C69" s="0">
-        <v>-20.418020258521835</v>
-      </c>
-      <c r="D69" s="0">
-        <v>-15.150890355136138</v>
+        <v>-15.084390270714625</v>
       </c>
     </row>
     <row r="70">
@@ -1053,13 +842,10 @@
         <v>2020000000</v>
       </c>
       <c r="B70" s="0">
-        <v>11.034920954902255</v>
+        <v>11.031196539998025</v>
       </c>
       <c r="C70" s="0">
-        <v>-20.264271043867609</v>
-      </c>
-      <c r="D70" s="0">
-        <v>-15.749143600162848</v>
+        <v>-15.627506653201866</v>
       </c>
     </row>
     <row r="71">
@@ -1067,13 +853,10 @@
         <v>2035000000</v>
       </c>
       <c r="B71" s="0">
-        <v>10.977318063408712</v>
+        <v>10.975100648625778</v>
       </c>
       <c r="C71" s="0">
-        <v>-20.443737709146998</v>
-      </c>
-      <c r="D71" s="0">
-        <v>-16.049519168398611</v>
+        <v>-16.081203636210773</v>
       </c>
     </row>
     <row r="72">
@@ -1081,13 +864,10 @@
         <v>2050000000</v>
       </c>
       <c r="B72" s="0">
-        <v>11.065623353933631</v>
+        <v>11.05631416336483</v>
       </c>
       <c r="C72" s="0">
-        <v>-20.330916077987467</v>
-      </c>
-      <c r="D72" s="0">
-        <v>-15.355631346433842</v>
+        <v>-15.506087138992491</v>
       </c>
     </row>
     <row r="73">
@@ -1095,13 +875,10 @@
         <v>2065000000</v>
       </c>
       <c r="B73" s="0">
-        <v>11.134520622442214</v>
+        <v>11.140734793214595</v>
       </c>
       <c r="C73" s="0">
-        <v>-20.256445439703612</v>
-      </c>
-      <c r="D73" s="0">
-        <v>-15.887350336690783</v>
+        <v>-16.071850184947291</v>
       </c>
     </row>
     <row r="74">
@@ -1109,13 +886,10 @@
         <v>2080000000</v>
       </c>
       <c r="B74" s="0">
-        <v>11.227419879769567</v>
+        <v>11.229397745159025</v>
       </c>
       <c r="C74" s="0">
-        <v>-20.133512504455737</v>
-      </c>
-      <c r="D74" s="0">
-        <v>-16.767707681012325</v>
+        <v>-17.141905654171687</v>
       </c>
     </row>
     <row r="75">
@@ -1123,13 +897,10 @@
         <v>2095000000</v>
       </c>
       <c r="B75" s="0">
-        <v>11.289460156122873</v>
+        <v>11.284858857759684</v>
       </c>
       <c r="C75" s="0">
-        <v>-20.071845798540178</v>
-      </c>
-      <c r="D75" s="0">
-        <v>-16.447949860127146</v>
+        <v>-16.591337632798449</v>
       </c>
     </row>
     <row r="76">
@@ -1137,13 +908,10 @@
         <v>2110000000</v>
       </c>
       <c r="B76" s="0">
-        <v>11.361187445925447</v>
+        <v>11.354881813100429</v>
       </c>
       <c r="C76" s="0">
-        <v>-19.990359778842599</v>
-      </c>
-      <c r="D76" s="0">
-        <v>-17.406173857114165</v>
+        <v>-17.686115830867951</v>
       </c>
     </row>
     <row r="77">
@@ -1151,13 +919,10 @@
         <v>2125000000</v>
       </c>
       <c r="B77" s="0">
-        <v>11.398505426030811</v>
+        <v>11.395675230215955</v>
       </c>
       <c r="C77" s="0">
-        <v>-19.977253400404624</v>
-      </c>
-      <c r="D77" s="0">
-        <v>-19.204793776684753</v>
+        <v>-19.910510055895411</v>
       </c>
     </row>
     <row r="78">
@@ -1165,13 +930,10 @@
         <v>2140000000</v>
       </c>
       <c r="B78" s="0">
-        <v>11.465080172905859</v>
+        <v>11.460333058583576</v>
       </c>
       <c r="C78" s="0">
-        <v>-19.905200685911741</v>
-      </c>
-      <c r="D78" s="0">
-        <v>-20.468995412454703</v>
+        <v>-20.821245901433983</v>
       </c>
     </row>
     <row r="79">
@@ -1179,13 +941,10 @@
         <v>2155000000</v>
       </c>
       <c r="B79" s="0">
-        <v>11.508090179406057</v>
+        <v>11.525849152705007</v>
       </c>
       <c r="C79" s="0">
-        <v>-19.879850695862537</v>
-      </c>
-      <c r="D79" s="0">
-        <v>-19.816024081944214</v>
+        <v>-20.172654374192387</v>
       </c>
     </row>
     <row r="80">
@@ -1193,13 +952,10 @@
         <v>2170000000</v>
       </c>
       <c r="B80" s="0">
-        <v>11.5506691602047</v>
+        <v>11.55293134298917</v>
       </c>
       <c r="C80" s="0">
-        <v>-19.854941921300831</v>
-      </c>
-      <c r="D80" s="0">
-        <v>-20.313340472911371</v>
+        <v>-21.051673062818878</v>
       </c>
     </row>
     <row r="81">
@@ -1207,13 +963,10 @@
         <v>2185000000</v>
       </c>
       <c r="B81" s="0">
-        <v>11.585847759339247</v>
+        <v>11.578881151813533</v>
       </c>
       <c r="C81" s="0">
-        <v>-19.844418872189959</v>
-      </c>
-      <c r="D81" s="0">
-        <v>-21.894483780952623</v>
+        <v>-22.488017504721999</v>
       </c>
     </row>
     <row r="82">
@@ -1221,13 +974,10 @@
         <v>2200000000</v>
       </c>
       <c r="B82" s="0">
-        <v>11.579644574903142</v>
+        <v>11.577519718770198</v>
       </c>
       <c r="C82" s="0">
-        <v>-19.91625003137748</v>
-      </c>
-      <c r="D82" s="0">
-        <v>-19.248587254254168</v>
+        <v>-19.670433299702612</v>
       </c>
     </row>
     <row r="83">
@@ -1235,13 +985,10 @@
         <v>2215000000</v>
       </c>
       <c r="B83" s="0">
-        <v>11.582846332735949</v>
+        <v>11.557924021087565</v>
       </c>
       <c r="C83" s="0">
-        <v>-19.96886751044951</v>
-      </c>
-      <c r="D83" s="0">
-        <v>-15.858132182096883</v>
+        <v>-16.138153980193401</v>
       </c>
     </row>
     <row r="84">
@@ -1249,13 +996,10 @@
         <v>2230000000</v>
       </c>
       <c r="B84" s="0">
-        <v>11.547940860078556</v>
+        <v>11.555080742847579</v>
       </c>
       <c r="C84" s="0">
-        <v>-20.097301105545743</v>
-      </c>
-      <c r="D84" s="0">
-        <v>-16.115653231825874</v>
+        <v>-16.216672574471296</v>
       </c>
     </row>
     <row r="85">
@@ -1263,13 +1007,10 @@
         <v>2245000000</v>
       </c>
       <c r="B85" s="0">
-        <v>11.552772881095965</v>
+        <v>11.568247397890008</v>
       </c>
       <c r="C85" s="0">
-        <v>-20.145866709334548</v>
-      </c>
-      <c r="D85" s="0">
-        <v>-15.457982670679213</v>
+        <v>-15.804243414935165</v>
       </c>
     </row>
     <row r="86">
@@ -1277,13 +1018,10 @@
         <v>2260000000</v>
       </c>
       <c r="B86" s="0">
-        <v>11.54098253778518</v>
+        <v>11.535634336502046</v>
       </c>
       <c r="C86" s="0">
-        <v>-20.227289272117304</v>
-      </c>
-      <c r="D86" s="0">
-        <v>-13.127992450354157</v>
+        <v>-13.248474419497917</v>
       </c>
     </row>
     <row r="87">
@@ -1291,13 +1029,10 @@
         <v>2275000000</v>
       </c>
       <c r="B87" s="0">
-        <v>11.566270282903854</v>
+        <v>11.581226763238691</v>
       </c>
       <c r="C87" s="0">
-        <v>-20.234173018794557</v>
-      </c>
-      <c r="D87" s="0">
-        <v>-13.070358545017292</v>
+        <v>-12.923682880772871</v>
       </c>
     </row>
     <row r="88">
@@ -1305,13 +1040,10 @@
         <v>2290000000</v>
       </c>
       <c r="B88" s="0">
-        <v>11.539057027307159</v>
+        <v>11.554069313842177</v>
       </c>
       <c r="C88" s="0">
-        <v>-20.345681156923078</v>
-      </c>
-      <c r="D88" s="0">
-        <v>-13.67092788025227</v>
+        <v>-13.863033859580325</v>
       </c>
     </row>
     <row r="89">
@@ -1319,13 +1051,10 @@
         <v>2305000000</v>
       </c>
       <c r="B89" s="0">
-        <v>11.532633644852565</v>
+        <v>11.550242491964941</v>
       </c>
       <c r="C89" s="0">
-        <v>-20.415236869547858</v>
-      </c>
-      <c r="D89" s="0">
-        <v>-12.793836553028498</v>
+        <v>-12.913270492984294</v>
       </c>
     </row>
     <row r="90">
@@ -1333,13 +1062,10 @@
         <v>2320000000</v>
       </c>
       <c r="B90" s="0">
-        <v>11.518737535803956</v>
+        <v>11.5129575874649</v>
       </c>
       <c r="C90" s="0">
-        <v>-20.499370190949723</v>
-      </c>
-      <c r="D90" s="0">
-        <v>-12.502077953757398</v>
+        <v>-12.37087593941839</v>
       </c>
     </row>
     <row r="91">
@@ -1347,13 +1073,10 @@
         <v>2335000000</v>
       </c>
       <c r="B91" s="0">
-        <v>11.540036534287967</v>
+        <v>11.538316377974972</v>
       </c>
       <c r="C91" s="0">
-        <v>-20.512750194206326</v>
-      </c>
-      <c r="D91" s="0">
-        <v>-13.697352814740483</v>
+        <v>-13.744804923090721</v>
       </c>
     </row>
     <row r="92">
@@ -1361,13 +1084,10 @@
         <v>2350000000</v>
       </c>
       <c r="B92" s="0">
-        <v>11.470791642212852</v>
+        <v>11.479318986310776</v>
       </c>
       <c r="C92" s="0">
-        <v>-20.706859525748662</v>
-      </c>
-      <c r="D92" s="0">
-        <v>-14.275813266539112</v>
+        <v>-14.584051507651125</v>
       </c>
     </row>
     <row r="93">
@@ -1375,13 +1095,10 @@
         <v>2365000000</v>
       </c>
       <c r="B93" s="0">
-        <v>11.421433990274316</v>
+        <v>11.433614293329136</v>
       </c>
       <c r="C93" s="0">
-        <v>-20.860840485667623</v>
-      </c>
-      <c r="D93" s="0">
-        <v>-13.627301995447292</v>
+        <v>-13.472591336470421</v>
       </c>
     </row>
     <row r="94">
@@ -1389,13 +1106,10 @@
         <v>2380000000</v>
       </c>
       <c r="B94" s="0">
-        <v>11.321479117363833</v>
+        <v>11.318249142798024</v>
       </c>
       <c r="C94" s="0">
-        <v>-21.11566647114222</v>
-      </c>
-      <c r="D94" s="0">
-        <v>-14.023094759606444</v>
+        <v>-13.969889784951821</v>
       </c>
     </row>
     <row r="95">
@@ -1403,13 +1117,10 @@
         <v>2395000000</v>
       </c>
       <c r="B95" s="0">
-        <v>11.226555883891953</v>
+        <v>11.222153566783483</v>
       </c>
       <c r="C95" s="0">
-        <v>-21.360084151967374</v>
-      </c>
-      <c r="D95" s="0">
-        <v>-15.055070544300516</v>
+        <v>-15.505728325136708</v>
       </c>
     </row>
     <row r="96">
@@ -1417,13 +1128,10 @@
         <v>2410000000</v>
       </c>
       <c r="B96" s="0">
-        <v>11.053431291891336</v>
+        <v>11.045109274354452</v>
       </c>
       <c r="C96" s="0">
-        <v>-21.760563832454338</v>
-      </c>
-      <c r="D96" s="0">
-        <v>-13.486907066498606</v>
+        <v>-13.373591118654915</v>
       </c>
     </row>
     <row r="97">
@@ -1431,13 +1139,10 @@
         <v>2425000000</v>
       </c>
       <c r="B97" s="0">
-        <v>10.823162990532612</v>
+        <v>10.822664837808375</v>
       </c>
       <c r="C97" s="0">
-        <v>-22.274994442440068</v>
-      </c>
-      <c r="D97" s="0">
-        <v>-12.192349234323723</v>
+        <v>-11.997110902101443</v>
       </c>
     </row>
     <row r="98">
@@ -1445,13 +1150,10 @@
         <v>2440000000</v>
       </c>
       <c r="B98" s="0">
-        <v>10.629254468535756</v>
+        <v>10.630572512312575</v>
       </c>
       <c r="C98" s="0">
-        <v>-22.716373154442721</v>
-      </c>
-      <c r="D98" s="0">
-        <v>-11.7953958104296</v>
+        <v>-12.099876543997375</v>
       </c>
     </row>
     <row r="99">
@@ -1459,13 +1161,10 @@
         <v>2455000000</v>
       </c>
       <c r="B99" s="0">
-        <v>10.374416030314199</v>
+        <v>10.376365244458729</v>
       </c>
       <c r="C99" s="0">
-        <v>-23.279283433290988</v>
-      </c>
-      <c r="D99" s="0">
-        <v>-10.537117998823417</v>
+        <v>-10.379641226899082</v>
       </c>
     </row>
     <row r="100">
@@ -1473,13 +1172,10 @@
         <v>2470000000</v>
       </c>
       <c r="B100" s="0">
-        <v>10.040801012645026</v>
+        <v>10.089201768913435</v>
       </c>
       <c r="C100" s="0">
-        <v>-23.999422604642902</v>
-      </c>
-      <c r="D100" s="0">
-        <v>-9.3766314508319475</v>
+        <v>-9.2378485311558158</v>
       </c>
     </row>
     <row r="101">
@@ -1487,13 +1183,10 @@
         <v>2485000000</v>
       </c>
       <c r="B101" s="0">
-        <v>9.7643179801346349</v>
+        <v>9.7715863685697482</v>
       </c>
       <c r="C101" s="0">
-        <v>-24.604977465857395</v>
-      </c>
-      <c r="D101" s="0">
-        <v>-9.1992224192362286</v>
+        <v>-9.4009311130645656</v>
       </c>
     </row>
     <row r="102">
@@ -1501,13 +1194,10 @@
         <v>2500000000</v>
       </c>
       <c r="B102" s="0">
-        <v>9.4667997366017929</v>
+        <v>9.4765513927993172</v>
       </c>
       <c r="C102" s="0">
-        <v>-25.252286264976817</v>
-      </c>
-      <c r="D102" s="0">
-        <v>-8.6109331375794653</v>
+        <v>-8.407226175825862</v>
       </c>
     </row>
     <row r="103">
@@ -1515,13 +1205,10 @@
         <v>2515000000</v>
       </c>
       <c r="B103" s="0">
-        <v>9.1359168451169648</v>
+        <v>9.1654347265864864</v>
       </c>
       <c r="C103" s="0">
-        <v>-25.966011662344645</v>
-      </c>
-      <c r="D103" s="0">
-        <v>-8.2685005300134851</v>
+        <v>-8.2768878911235717</v>
       </c>
     </row>
     <row r="104">
@@ -1529,13 +1216,10 @@
         <v>2530000000</v>
       </c>
       <c r="B104" s="0">
-        <v>8.8910290628899631</v>
+        <v>8.8951211045780259</v>
       </c>
       <c r="C104" s="0">
-        <v>-26.507437862476074</v>
-      </c>
-      <c r="D104" s="0">
-        <v>-8.3387771477057751</v>
+        <v>-8.5248999288800782</v>
       </c>
     </row>
     <row r="105">
@@ -1543,13 +1227,10 @@
         <v>2545000000</v>
       </c>
       <c r="B105" s="0">
-        <v>8.6117971115108496</v>
+        <v>8.5752225561494431</v>
       </c>
       <c r="C105" s="0">
-        <v>-27.117247075173488</v>
-      </c>
-      <c r="D105" s="0">
-        <v>-8.6944271875875287</v>
+        <v>-8.4628474078807816</v>
       </c>
     </row>
     <row r="106">
@@ -1557,13 +1238,10 @@
         <v>2560000000</v>
       </c>
       <c r="B106" s="0">
-        <v>8.2778393560223904</v>
+        <v>8.3014010398783267</v>
       </c>
       <c r="C106" s="0">
-        <v>-27.836206158931851</v>
-      </c>
-      <c r="D106" s="0">
-        <v>-8.7743749551517762</v>
+        <v>-8.8387938842869431</v>
       </c>
     </row>
     <row r="107">
@@ -1571,13 +1249,10 @@
         <v>2575000000</v>
       </c>
       <c r="B107" s="0">
-        <v>7.9063731415166121</v>
+        <v>7.908105928856024</v>
       </c>
       <c r="C107" s="0">
-        <v>-28.629883949250615</v>
-      </c>
-      <c r="D107" s="0">
-        <v>-9.6685168544993942</v>
+        <v>-9.8203582212099843</v>
       </c>
     </row>
     <row r="108">
@@ -1585,13 +1260,10 @@
         <v>2590000000</v>
       </c>
       <c r="B108" s="0">
-        <v>7.4275111154891569</v>
+        <v>7.4612317934304251</v>
       </c>
       <c r="C108" s="0">
-        <v>-29.638058615386363</v>
-      </c>
-      <c r="D108" s="0">
-        <v>-10.887953304175134</v>
+        <v>-10.57316400383456</v>
       </c>
     </row>
     <row r="109">
@@ -1599,13 +1271,10 @@
         <v>2605000000</v>
       </c>
       <c r="B109" s="0">
-        <v>6.8335811696566129</v>
+        <v>6.8256480422483161</v>
       </c>
       <c r="C109" s="0">
-        <v>-30.876077778137283</v>
-      </c>
-      <c r="D109" s="0">
-        <v>-10.537221795614704</v>
+        <v>-10.56436931430666</v>
       </c>
     </row>
     <row r="110">
@@ -1613,13 +1282,10 @@
         <v>2620000000</v>
       </c>
       <c r="B110" s="0">
-        <v>6.0689663801414007</v>
+        <v>6.0804665952257686</v>
       </c>
       <c r="C110" s="0">
-        <v>-32.455178630851755</v>
-      </c>
-      <c r="D110" s="0">
-        <v>-9.7465765117831342</v>
+        <v>-9.8219078993673943</v>
       </c>
     </row>
     <row r="111">
@@ -1627,13 +1293,10 @@
         <v>2635000000</v>
       </c>
       <c r="B111" s="0">
-        <v>5.207545974603299</v>
+        <v>5.2348326372048248</v>
       </c>
       <c r="C111" s="0">
-        <v>-34.227606006504352</v>
-      </c>
-      <c r="D111" s="0">
-        <v>-9.5631965016882035</v>
+        <v>-9.4037939876365257</v>
       </c>
     </row>
     <row r="112">
@@ -1641,13 +1304,10 @@
         <v>2650000000</v>
       </c>
       <c r="B112" s="0">
-        <v>4.281456506037955</v>
+        <v>4.3189535010424507</v>
       </c>
       <c r="C112" s="0">
-        <v>-36.12909003139989</v>
-      </c>
-      <c r="D112" s="0">
-        <v>-8.4221789851178741</v>
+        <v>-8.471287928235645</v>
       </c>
     </row>
     <row r="113">
@@ -1655,13 +1315,10 @@
         <v>2665000000</v>
       </c>
       <c r="B113" s="0">
-        <v>3.2477634416468746</v>
+        <v>3.1672845482029537</v>
       </c>
       <c r="C113" s="0">
-        <v>-38.245502948697712</v>
-      </c>
-      <c r="D113" s="0">
-        <v>-7.2473132302505094</v>
+        <v>-7.1993836690405209</v>
       </c>
     </row>
     <row r="114">
@@ -1669,13 +1326,10 @@
         <v>2680000000</v>
       </c>
       <c r="B114" s="0">
-        <v>2.1948805445557191</v>
+        <v>2.1186760700697214</v>
       </c>
       <c r="C114" s="0">
-        <v>-40.400020356203981</v>
-      </c>
-      <c r="D114" s="0">
-        <v>-7.1557557912461736</v>
+        <v>-7.0702573812385161</v>
       </c>
     </row>
     <row r="115">
@@ -1683,13 +1337,10 @@
         <v>2695000000</v>
       </c>
       <c r="B115" s="0">
-        <v>1.0911700199322532</v>
+        <v>1.1256527382703609</v>
       </c>
       <c r="C115" s="0">
-        <v>-42.655920915330285</v>
-      </c>
-      <c r="D115" s="0">
-        <v>-6.9134621821821991</v>
+        <v>-7.0346411849698276</v>
       </c>
     </row>
     <row r="116">
@@ -1697,13 +1348,10 @@
         <v>2710000000</v>
       </c>
       <c r="B116" s="0">
-        <v>-0.10704357255967523</v>
+        <v>-0.06887450920786975</v>
       </c>
       <c r="C116" s="0">
-        <v>-45.100558527347104</v>
-      </c>
-      <c r="D116" s="0">
-        <v>-6.7023479342056831</v>
+        <v>-6.5456817488501331</v>
       </c>
     </row>
     <row r="117">
@@ -1711,13 +1359,10 @@
         <v>2725000000</v>
       </c>
       <c r="B117" s="0">
-        <v>-1.2388000219310307</v>
+        <v>-1.313648098712271</v>
       </c>
       <c r="C117" s="0">
-        <v>-47.412015740854926</v>
-      </c>
-      <c r="D117" s="0">
-        <v>-7.140823663092041</v>
+        <v>-7.036753750654194</v>
       </c>
     </row>
     <row r="118">
@@ -1725,13 +1370,10 @@
         <v>2740000000</v>
       </c>
       <c r="B118" s="0">
-        <v>-2.0573051867047703</v>
+        <v>-1.6967428391560411</v>
       </c>
       <c r="C118" s="0">
-        <v>-49.096707194556942</v>
-      </c>
-      <c r="D118" s="0">
-        <v>-7.9688190101773166</v>
+        <v>-8.1553005518193995</v>
       </c>
     </row>
     <row r="119">
@@ -1739,13 +1381,10 @@
         <v>2755000000</v>
       </c>
       <c r="B119" s="0">
-        <v>-2.5949707664572443</v>
+        <v>-2.8759238658219815</v>
       </c>
       <c r="C119" s="0">
-        <v>-50.219459161410214</v>
-      </c>
-      <c r="D119" s="0">
-        <v>-8.7056710428662392</v>
+        <v>-8.4626924446516565</v>
       </c>
     </row>
     <row r="120">
@@ -1753,13 +1392,10 @@
         <v>2770000000</v>
       </c>
       <c r="B120" s="0">
-        <v>-2.6108369302335603</v>
+        <v>-2.2025792407474647</v>
       </c>
       <c r="C120" s="0">
-        <v>-50.298354806495738</v>
-      </c>
-      <c r="D120" s="0">
-        <v>-9.0792562818827722</v>
+        <v>-8.9521397505174818</v>
       </c>
     </row>
     <row r="121">
@@ -1767,13 +1403,10 @@
         <v>2785000000</v>
       </c>
       <c r="B121" s="0">
-        <v>-2.5529620092222984</v>
+        <v>-2.4427986678480522</v>
       </c>
       <c r="C121" s="0">
-        <v>-50.229513573379201</v>
-      </c>
-      <c r="D121" s="0">
-        <v>-9.1794547312262544</v>
+        <v>-9.4542108738854793</v>
       </c>
     </row>
     <row r="122">
@@ -1781,13 +1414,10 @@
         <v>2800000000</v>
       </c>
       <c r="B122" s="0">
-        <v>-2.3382044168332712</v>
+        <v>-2.3801508200652677</v>
       </c>
       <c r="C122" s="0">
-        <v>-49.84665502525057</v>
-      </c>
-      <c r="D122" s="0">
-        <v>-8.847345822475468</v>
+        <v>-8.6987930312586847</v>
       </c>
     </row>
     <row r="123">
@@ -1795,13 +1425,10 @@
         <v>2815000000</v>
       </c>
       <c r="B123" s="0">
-        <v>-2.5758962136762946</v>
+        <v>-2.4356387221833593</v>
       </c>
       <c r="C123" s="0">
-        <v>-50.368445975839535</v>
-      </c>
-      <c r="D123" s="0">
-        <v>-7.6079659427414414</v>
+        <v>-7.4847905027270345</v>
       </c>
     </row>
     <row r="124">
@@ -1809,13 +1436,10 @@
         <v>2830000000</v>
       </c>
       <c r="B124" s="0">
-        <v>-2.1916877430929773</v>
+        <v>-1.6718316151678074</v>
       </c>
       <c r="C124" s="0">
-        <v>-49.646189761411399</v>
-      </c>
-      <c r="D124" s="0">
-        <v>-6.992699397226648</v>
+        <v>-7.2129939770349152</v>
       </c>
     </row>
     <row r="125">
@@ -1823,13 +1447,10 @@
         <v>2845000000</v>
       </c>
       <c r="B125" s="0">
-        <v>-1.5987602665683198</v>
+        <v>-1.7359121412556497</v>
       </c>
       <c r="C125" s="0">
-        <v>-48.506251512498082</v>
-      </c>
-      <c r="D125" s="0">
-        <v>-7.0370057423177279</v>
+        <v>-6.9246942542209498</v>
       </c>
     </row>
     <row r="126">
@@ -1837,13 +1458,10 @@
         <v>2860000000</v>
       </c>
       <c r="B126" s="0">
-        <v>-0.4928021190606664</v>
+        <v>-0.39762324542302352</v>
       </c>
       <c r="C126" s="0">
-        <v>-46.340010465441836</v>
-      </c>
-      <c r="D126" s="0">
-        <v>-7.0189198481074078</v>
+        <v>-6.9226725322389342</v>
       </c>
     </row>
     <row r="127">
@@ -1851,13 +1469,10 @@
         <v>2875000000</v>
       </c>
       <c r="B127" s="0">
-        <v>0.48492277864805189</v>
+        <v>0.56687720881945225</v>
       </c>
       <c r="C127" s="0">
-        <v>-44.429996987956521</v>
-      </c>
-      <c r="D127" s="0">
-        <v>-7.1542832630507824</v>
+        <v>-7.3731839921240621</v>
       </c>
     </row>
     <row r="128">
@@ -1865,13 +1480,10 @@
         <v>2890000000</v>
       </c>
       <c r="B128" s="0">
-        <v>1.5497432704282801</v>
+        <v>1.5676158234643012</v>
       </c>
       <c r="C128" s="0">
-        <v>-42.345555879014036</v>
-      </c>
-      <c r="D128" s="0">
-        <v>-7.9839048529851722</v>
+        <v>-7.7430341614057498</v>
       </c>
     </row>
     <row r="129">
@@ -1879,13 +1491,10 @@
         <v>2905000000</v>
       </c>
       <c r="B129" s="0">
-        <v>2.1631822293836294</v>
+        <v>2.2689546073216498</v>
       </c>
       <c r="C129" s="0">
-        <v>-41.163643840499375</v>
-      </c>
-      <c r="D129" s="0">
-        <v>-9.4457235223030835</v>
+        <v>-9.3405086861825168</v>
       </c>
     </row>
     <row r="130">
@@ -1893,13 +1502,10 @@
         <v>2920000000</v>
       </c>
       <c r="B130" s="0">
-        <v>2.6925054261131862</v>
+        <v>2.6709533687781395</v>
       </c>
       <c r="C130" s="0">
-        <v>-40.149731741481638</v>
-      </c>
-      <c r="D130" s="0">
-        <v>-9.3416310264229345</v>
+        <v>-9.69366588026854</v>
       </c>
     </row>
     <row r="131">
@@ -1907,13 +1513,10 @@
         <v>2935000000</v>
       </c>
       <c r="B131" s="0">
-        <v>2.7304881030690105</v>
+        <v>2.6723643811385074</v>
       </c>
       <c r="C131" s="0">
-        <v>-40.118271470274287</v>
-      </c>
-      <c r="D131" s="0">
-        <v>-8.0552338246613555</v>
+        <v>-7.8859615052706422</v>
       </c>
     </row>
     <row r="132">
@@ -1921,13 +1524,10 @@
         <v>2950000000</v>
       </c>
       <c r="B132" s="0">
-        <v>2.7228768298069781</v>
+        <v>2.7386623704713031</v>
       </c>
       <c r="C132" s="0">
-        <v>-40.177772224688944</v>
-      </c>
-      <c r="D132" s="0">
-        <v>-7.5092540081439392</v>
+        <v>-7.2926865299411947</v>
       </c>
     </row>
     <row r="133">
@@ -1935,13 +1535,10 @@
         <v>2965000000</v>
       </c>
       <c r="B133" s="0">
-        <v>2.8106164256614932</v>
+        <v>2.7693866046741888</v>
       </c>
       <c r="C133" s="0">
-        <v>-40.046346667422284</v>
-      </c>
-      <c r="D133" s="0">
-        <v>-7.1070187896997368</v>
+        <v>-7.4268692565244301</v>
       </c>
     </row>
     <row r="134">
@@ -1949,13 +1546,10 @@
         <v>2980000000</v>
       </c>
       <c r="B134" s="0">
-        <v>3.0730240414340706</v>
+        <v>3.1172901130670674</v>
       </c>
       <c r="C134" s="0">
-        <v>-39.565362763396607</v>
-      </c>
-      <c r="D134" s="0">
-        <v>-6.2833251080624226</v>
+        <v>-6.113092262781608</v>
       </c>
     </row>
     <row r="135">
@@ -1963,13 +1557,10 @@
         <v>2995000000</v>
       </c>
       <c r="B135" s="0">
-        <v>3.4647526618581637</v>
+        <v>3.4462199035535548</v>
       </c>
       <c r="C135" s="0">
-        <v>-38.82551677552992</v>
-      </c>
-      <c r="D135" s="0">
-        <v>-6.839479757248518</v>
+        <v>-6.6625472619057007</v>
       </c>
     </row>
     <row r="136">
@@ -1977,13 +1568,10 @@
         <v>3010000000</v>
       </c>
       <c r="B136" s="0">
-        <v>4.204615941695991</v>
+        <v>4.1497833642205038</v>
       </c>
       <c r="C136" s="0">
-        <v>-37.38918359322453</v>
-      </c>
-      <c r="D136" s="0">
-        <v>-8.2600837026585801</v>
+        <v>-8.5552687760789166</v>
       </c>
     </row>
     <row r="137">
@@ -1991,13 +1579,10 @@
         <v>3025000000</v>
       </c>
       <c r="B137" s="0">
-        <v>4.1234082130484246</v>
+        <v>4.0928566922037781</v>
       </c>
       <c r="C137" s="0">
-        <v>-37.594776718412547</v>
-      </c>
-      <c r="D137" s="0">
-        <v>-9.9815329814227312</v>
+        <v>-9.8186859449846438</v>
       </c>
     </row>
     <row r="138">
@@ -2005,13 +1590,10 @@
         <v>3040000000</v>
       </c>
       <c r="B138" s="0">
-        <v>3.0612967809275275</v>
+        <v>3.0171088612426615</v>
       </c>
       <c r="C138" s="0">
-        <v>-39.761963675059661</v>
-      </c>
-      <c r="D138" s="0">
-        <v>-9.6462754966126969</v>
+        <v>-9.4103022867846562</v>
       </c>
     </row>
     <row r="139">
@@ -2019,13 +1601,10 @@
         <v>3055000000</v>
       </c>
       <c r="B139" s="0">
-        <v>1.6840300137071296</v>
+        <v>1.755393005188445</v>
       </c>
       <c r="C139" s="0">
-        <v>-42.559249828896846</v>
-      </c>
-      <c r="D139" s="0">
-        <v>-8.5174835761518111</v>
+        <v>-8.6365475933140488</v>
       </c>
     </row>
     <row r="140">
@@ -2033,13 +1612,10 @@
         <v>3070000000</v>
       </c>
       <c r="B140" s="0">
-        <v>0.44931180649258451</v>
+        <v>0.50087336381299608</v>
       </c>
       <c r="C140" s="0">
-        <v>-45.071229461298202</v>
-      </c>
-      <c r="D140" s="0">
-        <v>-7.4088999069932369</v>
+        <v>-7.4268882534759664</v>
       </c>
     </row>
     <row r="141">
@@ -2047,13 +1623,10 @@
         <v>3085000000</v>
       </c>
       <c r="B141" s="0">
-        <v>-0.22060023052054589</v>
+        <v>0.0035211808753778939</v>
       </c>
       <c r="C141" s="0">
-        <v>-46.453389393165935</v>
-      </c>
-      <c r="D141" s="0">
-        <v>-6.5035984189664617</v>
+        <v>-6.4834400469100562</v>
       </c>
     </row>
     <row r="142">
@@ -2061,13 +1634,10 @@
         <v>3100000000</v>
       </c>
       <c r="B142" s="0">
-        <v>0.39609073749311463</v>
+        <v>0.049275073042277739</v>
       </c>
       <c r="C142" s="0">
-        <v>-45.262137966438864</v>
-      </c>
-      <c r="D142" s="0">
-        <v>-7.0391801000042475</v>
+        <v>-7.0712780538209632</v>
       </c>
     </row>
     <row r="143">
@@ -2075,13 +1645,10 @@
         <v>3115000000</v>
       </c>
       <c r="B143" s="0">
-        <v>0.66946921420944605</v>
+        <v>0.54493990917727331</v>
       </c>
       <c r="C143" s="0">
-        <v>-44.757308156224518</v>
-      </c>
-      <c r="D143" s="0">
-        <v>-9.9369889777633418</v>
+        <v>-9.9721367555229978</v>
       </c>
     </row>
     <row r="144">
@@ -2089,13 +1656,10 @@
         <v>3130000000</v>
       </c>
       <c r="B144" s="0">
-        <v>-0.17996036914560776</v>
+        <v>0.31015804927016788</v>
       </c>
       <c r="C144" s="0">
-        <v>-46.497893053959835</v>
-      </c>
-      <c r="D144" s="0">
-        <v>-12.456388009517216</v>
+        <v>-12.639470989151091</v>
       </c>
     </row>
     <row r="145">
@@ -2103,13 +1667,10 @@
         <v>3145000000</v>
       </c>
       <c r="B145" s="0">
-        <v>-0.29674953079398136</v>
+        <v>-0.39930352441988148</v>
       </c>
       <c r="C145" s="0">
-        <v>-46.772997621953358</v>
-      </c>
-      <c r="D145" s="0">
-        <v>-9.6410162187660617</v>
+        <v>-9.6443184597344001</v>
       </c>
     </row>
     <row r="146">
@@ -2117,13 +1678,10 @@
         <v>3160000000</v>
       </c>
       <c r="B146" s="0">
-        <v>-1.0255074377735873</v>
+        <v>-1.0943328002233379</v>
       </c>
       <c r="C146" s="0">
-        <v>-48.271842092654893</v>
-      </c>
-      <c r="D146" s="0">
-        <v>-8.1243567832819785</v>
+        <v>-8.0181862929010208</v>
       </c>
     </row>
     <row r="147">
@@ -2131,13 +1689,10 @@
         <v>3175000000</v>
       </c>
       <c r="B147" s="0">
-        <v>-1.2612469695069706</v>
+        <v>-1.0010484801303861</v>
       </c>
       <c r="C147" s="0">
-        <v>-48.784454096313475</v>
-      </c>
-      <c r="D147" s="0">
-        <v>-7.068862615694286</v>
+        <v>-7.1448422695596747</v>
       </c>
     </row>
     <row r="148">
@@ -2145,13 +1700,10 @@
         <v>3190000000</v>
       </c>
       <c r="B148" s="0">
-        <v>-0.24836779662284414</v>
+        <v>-0.50993691796814389</v>
       </c>
       <c r="C148" s="0">
-        <v>-46.799634819128954</v>
-      </c>
-      <c r="D148" s="0">
-        <v>-7.6324328731751727</v>
+        <v>-7.5388323000270052</v>
       </c>
     </row>
     <row r="149">
@@ -2159,13 +1711,10 @@
         <v>3205000000</v>
       </c>
       <c r="B149" s="0">
-        <v>0.70638146783688782</v>
+        <v>0.84876858113626241</v>
       </c>
       <c r="C149" s="0">
-        <v>-44.930883306162592</v>
-      </c>
-      <c r="D149" s="0">
-        <v>-10.501292043196273</v>
+        <v>-10.401877796573181</v>
       </c>
     </row>
     <row r="150">
@@ -2173,13 +1722,10 @@
         <v>3220000000</v>
       </c>
       <c r="B150" s="0">
-        <v>1.4316710727364921</v>
+        <v>1.4177261928527152</v>
       </c>
       <c r="C150" s="0">
-        <v>-43.520860853183279</v>
-      </c>
-      <c r="D150" s="0">
-        <v>-15.241024825281315</v>
+        <v>-15.374673647834921</v>
       </c>
     </row>
     <row r="151">
@@ -2187,13 +1733,10 @@
         <v>3235000000</v>
       </c>
       <c r="B151" s="0">
-        <v>1.2176142210572358</v>
+        <v>0.9471807823337457</v>
       </c>
       <c r="C151" s="0">
-        <v>-43.989342822719557</v>
-      </c>
-      <c r="D151" s="0">
-        <v>-11.600469395620266</v>
+        <v>-11.54237325221734</v>
       </c>
     </row>
     <row r="152">
@@ -2201,13 +1744,10 @@
         <v>3250000000</v>
       </c>
       <c r="B152" s="0">
-        <v>0.17524809223083082</v>
+        <v>0.076510307871007655</v>
       </c>
       <c r="C152" s="0">
-        <v>-46.114256599855466</v>
-      </c>
-      <c r="D152" s="0">
-        <v>-9.0903776585895724</v>
+        <v>-9.0914055827970248</v>
       </c>
     </row>
     <row r="153">
@@ -2215,13 +1755,10 @@
         <v>3265000000</v>
       </c>
       <c r="B153" s="0">
-        <v>-0.7546829590656543</v>
+        <v>-0.23745115058484245</v>
       </c>
       <c r="C153" s="0">
-        <v>-48.014115195092813</v>
-      </c>
-      <c r="D153" s="0">
-        <v>-8.0077662591230716</v>
+        <v>-8.0468540884194013</v>
       </c>
     </row>
     <row r="154">
@@ -2229,13 +1766,10 @@
         <v>3280000000</v>
       </c>
       <c r="B154" s="0">
-        <v>-0.2621735136827148</v>
+        <v>0.19310082841275999</v>
       </c>
       <c r="C154" s="0">
-        <v>-47.068909466338653</v>
-      </c>
-      <c r="D154" s="0">
-        <v>-8.7653773941370758</v>
+        <v>-8.5915603969629846</v>
       </c>
     </row>
     <row r="155">
@@ -2243,13 +1777,10 @@
         <v>3295000000</v>
       </c>
       <c r="B155" s="0">
-        <v>0.28973188399573502</v>
+        <v>0.20794730793434368</v>
       </c>
       <c r="C155" s="0">
-        <v>-46.004730175348747</v>
-      </c>
-      <c r="D155" s="0">
-        <v>-13.220998885404917</v>
+        <v>-13.337001490725537</v>
       </c>
     </row>
     <row r="156">
@@ -2257,13 +1788,10 @@
         <v>3310000000</v>
       </c>
       <c r="B156" s="0">
-        <v>0.60652235267718169</v>
+        <v>0.68564966339675593</v>
       </c>
       <c r="C156" s="0">
-        <v>-45.410600734899653</v>
-      </c>
-      <c r="D156" s="0">
-        <v>-15.448186036973517</v>
+        <v>-15.904956007120237</v>
       </c>
     </row>
     <row r="157">
@@ -2271,13 +1799,10 @@
         <v>3325000000</v>
       </c>
       <c r="B157" s="0">
-        <v>-0.22238350064461088</v>
+        <v>0.040053634371812308</v>
       </c>
       <c r="C157" s="0">
-        <v>-47.10768555881134</v>
-      </c>
-      <c r="D157" s="0">
-        <v>-9.783012135667434</v>
+        <v>-9.6037727830464963</v>
       </c>
     </row>
     <row r="158">
@@ -2285,13 +1810,10 @@
         <v>3340000000</v>
       </c>
       <c r="B158" s="0">
-        <v>-0.57335164644768355</v>
+        <v>-0.65963233506101204</v>
       </c>
       <c r="C158" s="0">
-        <v>-47.848718193866297</v>
-      </c>
-      <c r="D158" s="0">
-        <v>-8.3465778945980826</v>
+        <v>-8.2420396268613239</v>
       </c>
     </row>
     <row r="159">
@@ -2299,13 +1821,10 @@
         <v>3355000000</v>
       </c>
       <c r="B159" s="0">
-        <v>-0.92054415389600663</v>
+        <v>-0.96990058135595802</v>
       </c>
       <c r="C159" s="0">
-        <v>-48.58202436263187</v>
-      </c>
-      <c r="D159" s="0">
-        <v>-9.0060129808626037</v>
+        <v>-9.212195976762878</v>
       </c>
     </row>
     <row r="160">
@@ -2313,13 +1832,10 @@
         <v>3370000000</v>
       </c>
       <c r="B160" s="0">
-        <v>-0.92720982745328229</v>
+        <v>-1.0553170011748989</v>
       </c>
       <c r="C160" s="0">
-        <v>-48.634103237072978</v>
-      </c>
-      <c r="D160" s="0">
-        <v>-9.2848157602572581</v>
+        <v>-8.9614535757161633</v>
       </c>
     </row>
     <row r="161">
@@ -2327,13 +1843,10 @@
         <v>3385000000</v>
       </c>
       <c r="B161" s="0">
-        <v>-0.40866998050592684</v>
+        <v>-0.49319114985857837</v>
       </c>
       <c r="C161" s="0">
-        <v>-47.635598986174763</v>
-      </c>
-      <c r="D161" s="0">
-        <v>-11.250373381805863</v>
+        <v>-11.020560538842993</v>
       </c>
     </row>
     <row r="162">
@@ -2341,13 +1854,10 @@
         <v>3400000000</v>
       </c>
       <c r="B162" s="0">
-        <v>-0.99820558414803173</v>
+        <v>-0.93891456468825041</v>
       </c>
       <c r="C162" s="0">
-        <v>-48.853075073880809</v>
-      </c>
-      <c r="D162" s="0">
-        <v>-12.119529968168841</v>
+        <v>-12.649038184110182</v>
       </c>
     </row>
     <row r="163">
@@ -2355,13 +1865,10 @@
         <v>3415000000</v>
       </c>
       <c r="B163" s="0">
-        <v>-1.6986958672062116</v>
+        <v>-2.545129156647608</v>
       </c>
       <c r="C163" s="0">
-        <v>-50.29229145950309</v>
-      </c>
-      <c r="D163" s="0">
-        <v>-8.9700141844170176</v>
+        <v>-8.9051532143385437</v>
       </c>
     </row>
     <row r="164">
@@ -2369,13 +1876,10 @@
         <v>3430000000</v>
       </c>
       <c r="B164" s="0">
-        <v>-2.8781838406657556</v>
+        <v>-3.2268866452439191</v>
       </c>
       <c r="C164" s="0">
-        <v>-52.689335646926565</v>
-      </c>
-      <c r="D164" s="0">
-        <v>-7.3323799715518412</v>
+        <v>-7.0754711453530215</v>
       </c>
     </row>
     <row r="165">
@@ -2383,13 +1887,10 @@
         <v>3445000000</v>
       </c>
       <c r="B165" s="0">
-        <v>-4.0209811693589863</v>
+        <v>-3.2626020028811702</v>
       </c>
       <c r="C165" s="0">
-        <v>-55.012832428330512</v>
-      </c>
-      <c r="D165" s="0">
-        <v>-7.876466066218609</v>
+        <v>-8.0337704273067008</v>
       </c>
     </row>
     <row r="166">
@@ -2397,13 +1898,10 @@
         <v>3460000000</v>
       </c>
       <c r="B166" s="0">
-        <v>-3.5698360835755452</v>
+        <v>-3.6493479051669091</v>
       </c>
       <c r="C166" s="0">
-        <v>-54.148279707746269</v>
-      </c>
-      <c r="D166" s="0">
-        <v>-8.1934952090552589</v>
+        <v>-8.0447601365697956</v>
       </c>
     </row>
     <row r="167">
@@ -2411,13 +1909,10 @@
         <v>3475000000</v>
       </c>
       <c r="B167" s="0">
-        <v>-5.639468302980184</v>
+        <v>-4.6044446115181543</v>
       </c>
       <c r="C167" s="0">
-        <v>-58.325118349222663</v>
-      </c>
-      <c r="D167" s="0">
-        <v>-7.6432144617045692</v>
+        <v>-7.5250005200755243</v>
       </c>
     </row>
     <row r="168">
@@ -2425,13 +1920,10 @@
         <v>3490000000</v>
       </c>
       <c r="B168" s="0">
-        <v>-5.5827967973870898</v>
+        <v>-4.9204160092815883</v>
       </c>
       <c r="C168" s="0">
-        <v>-58.249187698697426</v>
-      </c>
-      <c r="D168" s="0">
-        <v>-7.7513891107191863</v>
+        <v>-7.8432829780834501</v>
       </c>
     </row>
     <row r="169">
@@ -2439,13 +1931,10 @@
         <v>3505000000</v>
       </c>
       <c r="B169" s="0">
-        <v>-12.422722985157694</v>
+        <v>-8.3630647392889657</v>
       </c>
       <c r="C169" s="0">
-        <v>-71.966291981108583</v>
-      </c>
-      <c r="D169" s="0">
-        <v>-8.9023933736822709</v>
+        <v>-8.914014846057988</v>
       </c>
     </row>
     <row r="170">
@@ -2453,13 +1942,10 @@
         <v>3520000000</v>
       </c>
       <c r="B170" s="0">
-        <v>-8.5194870285647859</v>
+        <v>-8.3971069438227097</v>
       </c>
       <c r="C170" s="0">
-        <v>-64.196912891431836</v>
-      </c>
-      <c r="D170" s="0">
-        <v>-9.0583875788332353</v>
+        <v>-9.0174862014006472</v>
       </c>
     </row>
     <row r="171">
@@ -2467,13 +1953,10 @@
         <v>3535000000</v>
       </c>
       <c r="B171" s="0">
-        <v>-5.0063625594134464</v>
+        <v>-6.4476354084746923</v>
       </c>
       <c r="C171" s="0">
-        <v>-57.2075990462249</v>
-      </c>
-      <c r="D171" s="0">
-        <v>-9.9406846785398599</v>
+        <v>-9.9586035269443016</v>
       </c>
     </row>
     <row r="172">
@@ -2481,13 +1964,10 @@
         <v>3550000000</v>
       </c>
       <c r="B172" s="0">
-        <v>-7.9181153409829399</v>
+        <v>-7.0129127753133353</v>
       </c>
       <c r="C172" s="0">
-        <v>-63.067883307807406</v>
-      </c>
-      <c r="D172" s="0">
-        <v>-12.685080633164045</v>
+        <v>-12.711262424044138</v>
       </c>
     </row>
     <row r="173">
@@ -2495,13 +1975,10 @@
         <v>3565000000</v>
       </c>
       <c r="B173" s="0">
-        <v>-6.8537244288635861</v>
+        <v>-4.9713748139641822</v>
       </c>
       <c r="C173" s="0">
-        <v>-60.975725106224502</v>
-      </c>
-      <c r="D173" s="0">
-        <v>-13.046416319119471</v>
+        <v>-12.946526976015239</v>
       </c>
     </row>
     <row r="174">
@@ -2509,13 +1986,10 @@
         <v>3580000000</v>
       </c>
       <c r="B174" s="0">
-        <v>-8.1267462627986369</v>
+        <v>-9.1361597771994916</v>
       </c>
       <c r="C174" s="0">
-        <v>-63.558238623214407</v>
-      </c>
-      <c r="D174" s="0">
-        <v>-13.658536808219065</v>
+        <v>-13.795302071880295</v>
       </c>
     </row>
     <row r="175">
@@ -2523,13 +1997,10 @@
         <v>3595000000</v>
       </c>
       <c r="B175" s="0">
-        <v>-9.1026968757003601</v>
+        <v>-10.30343169756852</v>
       </c>
       <c r="C175" s="0">
-        <v>-65.546457210518398</v>
-      </c>
-      <c r="D175" s="0">
-        <v>-14.6614372402189</v>
+        <v>-14.501635111241239</v>
       </c>
     </row>
     <row r="176">
@@ -2537,13 +2008,10 @@
         <v>3610000000</v>
       </c>
       <c r="B176" s="0">
-        <v>-9.1107004019821076</v>
+        <v>-6.585622767121194</v>
       </c>
       <c r="C176" s="0">
-        <v>-65.598630406817023</v>
-      </c>
-      <c r="D176" s="0">
-        <v>-14.794154567161698</v>
+        <v>-14.686423701145007</v>
       </c>
     </row>
     <row r="177">
@@ -2551,13 +2019,10 @@
         <v>3625000000</v>
       </c>
       <c r="B177" s="0">
-        <v>-5.7901780810609154</v>
+        <v>-7.1023089263102079</v>
       </c>
       <c r="C177" s="0">
-        <v>-58.993601945001728</v>
-      </c>
-      <c r="D177" s="0">
-        <v>-14.660524648498042</v>
+        <v>-15.058695101024803</v>
       </c>
     </row>
     <row r="178">
@@ -2565,13 +2030,10 @@
         <v>3640000000</v>
       </c>
       <c r="B178" s="0">
-        <v>-4.5404095226097851</v>
+        <v>-5.191628238645869</v>
       </c>
       <c r="C178" s="0">
-        <v>-56.529932282940329</v>
-      </c>
-      <c r="D178" s="0">
-        <v>-15.248660749124266</v>
+        <v>-14.600530925324806</v>
       </c>
     </row>
     <row r="179">
@@ -2579,13 +2041,10 @@
         <v>3655000000</v>
       </c>
       <c r="B179" s="0">
-        <v>-4.8178032635570567</v>
+        <v>-4.4973008511207802</v>
       </c>
       <c r="C179" s="0">
-        <v>-57.120439717731344</v>
-      </c>
-      <c r="D179" s="0">
-        <v>-16.442662509904732</v>
+        <v>-16.266582539259666</v>
       </c>
     </row>
     <row r="180">
@@ -2593,13 +2052,10 @@
         <v>3670000000</v>
       </c>
       <c r="B180" s="0">
-        <v>-3.9713072114348833</v>
+        <v>-4.0125214867489483</v>
       </c>
       <c r="C180" s="0">
-        <v>-55.46302127265119</v>
-      </c>
-      <c r="D180" s="0">
-        <v>-16.270708590727008</v>
+        <v>-17.117543205698208</v>
       </c>
     </row>
     <row r="181">
@@ -2607,13 +2063,10 @@
         <v>3685000000</v>
       </c>
       <c r="B181" s="0">
-        <v>-4.6192029595924389</v>
+        <v>-4.0538005162289394</v>
       </c>
       <c r="C181" s="0">
-        <v>-56.794241327825929</v>
-      </c>
-      <c r="D181" s="0">
-        <v>-15.487823024856528</v>
+        <v>-14.501693408104543</v>
       </c>
     </row>
     <row r="182">
@@ -2621,13 +2074,10 @@
         <v>3700000000</v>
       </c>
       <c r="B182" s="0">
-        <v>-3.5721565403800781</v>
+        <v>-3.8802043942349869</v>
       </c>
       <c r="C182" s="0">
-        <v>-54.735433126839695</v>
-      </c>
-      <c r="D182" s="0">
-        <v>-16.58804591255171</v>
+        <v>-16.553499433985557</v>
       </c>
     </row>
     <row r="183">
@@ -2635,13 +2085,10 @@
         <v>3715000000</v>
       </c>
       <c r="B183" s="0">
-        <v>-3.0993954313917982</v>
+        <v>-2.6544725539122176</v>
       </c>
       <c r="C183" s="0">
-        <v>-53.825052789455121</v>
-      </c>
-      <c r="D183" s="0">
-        <v>-15.847002429592054</v>
+        <v>-16.694174066379965</v>
       </c>
     </row>
     <row r="184">
@@ -2649,13 +2096,10 @@
         <v>3730000000</v>
       </c>
       <c r="B184" s="0">
-        <v>-3.3438754892627998</v>
+        <v>-3.0912023552150174</v>
       </c>
       <c r="C184" s="0">
-        <v>-54.349013179438998</v>
-      </c>
-      <c r="D184" s="0">
-        <v>-14.774416691690785</v>
+        <v>-14.020040673760557</v>
       </c>
     </row>
     <row r="185">
@@ -2663,13 +2107,10 @@
         <v>3745000000</v>
       </c>
       <c r="B185" s="0">
-        <v>-3.677620064384449</v>
+        <v>-3.0925238531558286</v>
       </c>
       <c r="C185" s="0">
-        <v>-55.051362134218245</v>
-      </c>
-      <c r="D185" s="0">
-        <v>-14.81554668821769</v>
+        <v>-14.845328562139342</v>
       </c>
     </row>
     <row r="186">
@@ -2677,13 +2118,10 @@
         <v>3760000000</v>
       </c>
       <c r="B186" s="0">
-        <v>-3.4211201490189822</v>
+        <v>-2.9148112889721745</v>
       </c>
       <c r="C186" s="0">
-        <v>-54.573082761330831</v>
-      </c>
-      <c r="D186" s="0">
-        <v>-14.602286715922341</v>
+        <v>-15.173367233333925</v>
       </c>
     </row>
     <row r="187">
@@ -2691,13 +2129,10 @@
         <v>3775000000</v>
       </c>
       <c r="B187" s="0">
-        <v>-2.8211227224395223</v>
+        <v>-5.0422368555618142</v>
       </c>
       <c r="C187" s="0">
-        <v>-53.407670128922831</v>
-      </c>
-      <c r="D187" s="0">
-        <v>-14.776787688774746</v>
+        <v>-14.602715017537658</v>
       </c>
     </row>
     <row r="188">
@@ -2705,13 +2140,10 @@
         <v>3790000000</v>
       </c>
       <c r="B188" s="0">
-        <v>-4.480142037073179</v>
+        <v>-4.6515663726709988</v>
       </c>
       <c r="C188" s="0">
-        <v>-56.760153838247447</v>
-      </c>
-      <c r="D188" s="0">
-        <v>-14.285422141773584</v>
+        <v>-14.082963687518333</v>
       </c>
     </row>
     <row r="189">
@@ -2719,13 +2151,10 @@
         <v>3805000000</v>
       </c>
       <c r="B189" s="0">
-        <v>-3.0895247941495469</v>
+        <v>-3.7351442859655748</v>
       </c>
       <c r="C189" s="0">
-        <v>-54.01322837517057</v>
-      </c>
-      <c r="D189" s="0">
-        <v>-14.574168646865406</v>
+        <v>-14.544483247557086</v>
       </c>
     </row>
     <row r="190">
@@ -2733,13 +2162,10 @@
         <v>3820000000</v>
       </c>
       <c r="B190" s="0">
-        <v>-6.3299124495556143</v>
+        <v>-5.8656881855115444</v>
       </c>
       <c r="C190" s="0">
-        <v>-60.528177722085047</v>
-      </c>
-      <c r="D190" s="0">
-        <v>-14.751224781196829</v>
+        <v>-14.884529096475987</v>
       </c>
     </row>
     <row r="191">
@@ -2747,13 +2173,10 @@
         <v>3835000000</v>
       </c>
       <c r="B191" s="0">
-        <v>-5.7681823196539597</v>
+        <v>-5.9233270168711023</v>
       </c>
       <c r="C191" s="0">
-        <v>-59.438757569747558</v>
-      </c>
-      <c r="D191" s="0">
-        <v>-14.314462739827638</v>
+        <v>-14.183345009872127</v>
       </c>
     </row>
     <row r="192">
@@ -2761,13 +2184,10 @@
         <v>3850000000</v>
       </c>
       <c r="B192" s="0">
-        <v>-6.396050880989641</v>
+        <v>-5.9391225497391389</v>
       </c>
       <c r="C192" s="0">
-        <v>-60.728401916888934</v>
-      </c>
-      <c r="D192" s="0">
-        <v>-14.045996322738661</v>
+        <v>-13.804047489692417</v>
       </c>
     </row>
     <row r="193">
@@ -2775,13 +2195,10 @@
         <v>3865000000</v>
       </c>
       <c r="B193" s="0">
-        <v>-7.2500952176233966</v>
+        <v>-6.0109213023840304</v>
       </c>
       <c r="C193" s="0">
-        <v>-62.470265965073317</v>
-      </c>
-      <c r="D193" s="0">
-        <v>-13.571693963936401</v>
+        <v>-13.835943524120058</v>
       </c>
     </row>
     <row r="194">
@@ -2789,13 +2206,10 @@
         <v>3880000000</v>
       </c>
       <c r="B194" s="0">
-        <v>-6.4187879020165219</v>
+        <v>-6.6061305584576822</v>
       </c>
       <c r="C194" s="0">
-        <v>-60.84129588065683</v>
-      </c>
-      <c r="D194" s="0">
-        <v>-13.369109326123008</v>
+        <v>-13.446713148248621</v>
       </c>
     </row>
     <row r="195">
@@ -2803,13 +2217,10 @@
         <v>3895000000</v>
       </c>
       <c r="B195" s="0">
-        <v>-6.7424075961745906</v>
+        <v>-7.1478161048358615</v>
       </c>
       <c r="C195" s="0">
-        <v>-61.522049997260488</v>
-      </c>
-      <c r="D195" s="0">
-        <v>-13.891394590350718</v>
+        <v>-13.76720759864784</v>
       </c>
     </row>
     <row r="196">
@@ -2817,13 +2228,10 @@
         <v>3910000000</v>
       </c>
       <c r="B196" s="0">
-        <v>-7.1690496613376453</v>
+        <v>-6.1063562313680784</v>
       </c>
       <c r="C196" s="0">
-        <v>-62.408720035332273</v>
-      </c>
-      <c r="D196" s="0">
-        <v>-12.504949376872363</v>
+        <v>-12.379490463931495</v>
       </c>
     </row>
     <row r="197">
@@ -2831,13 +2239,10 @@
         <v>3925000000</v>
       </c>
       <c r="B197" s="0">
-        <v>-7.2309721748861158</v>
+        <v>-7.2238799894103138</v>
       </c>
       <c r="C197" s="0">
-        <v>-62.565823136137304</v>
-      </c>
-      <c r="D197" s="0">
-        <v>-13.344934067645225</v>
+        <v>-13.552586398982529</v>
       </c>
     </row>
     <row r="198">
@@ -2845,13 +2250,10 @@
         <v>3940000000</v>
       </c>
       <c r="B198" s="0">
-        <v>-7.1451867941304457</v>
+        <v>-10.695546306624863</v>
       </c>
       <c r="C198" s="0">
-        <v>-62.427383589512019</v>
-      </c>
-      <c r="D198" s="0">
-        <v>-15.217826268051976</v>
+        <v>-15.165224233098659</v>
       </c>
     </row>
     <row r="199">
@@ -2859,13 +2261,10 @@
         <v>3955000000</v>
       </c>
       <c r="B199" s="0">
-        <v>-12.683827500650789</v>
+        <v>-7.8105070749890579</v>
       </c>
       <c r="C199" s="0">
-        <v>-73.53767032271513</v>
-      </c>
-      <c r="D199" s="0">
-        <v>-13.198498132533711</v>
+        <v>-12.908442861007156</v>
       </c>
     </row>
     <row r="200">
@@ -2873,13 +2272,10 @@
         <v>3970000000</v>
       </c>
       <c r="B200" s="0">
-        <v>-9.8783601218006396</v>
+        <v>-7.744290155765551</v>
       </c>
       <c r="C200" s="0">
-        <v>-67.959615943603225</v>
-      </c>
-      <c r="D200" s="0">
-        <v>-13.4489298700726</v>
+        <v>-13.798535531182171</v>
       </c>
     </row>
     <row r="201">
@@ -2887,13 +2283,10 @@
         <v>3985000000</v>
       </c>
       <c r="B201" s="0">
-        <v>-10.438587273915591</v>
+        <v>-15.178357321338805</v>
       </c>
       <c r="C201" s="0">
-        <v>-69.112826627213451</v>
-      </c>
-      <c r="D201" s="0">
-        <v>-15.573982407762228</v>
+        <v>-15.58329295768289</v>
       </c>
     </row>
     <row r="202">
@@ -2901,13 +2294,10 @@
         <v>4000000000</v>
       </c>
       <c r="B202" s="0">
-        <v>-9.717273972745808</v>
+        <v>-13.04473494610928</v>
       </c>
       <c r="C202" s="0">
-        <v>-67.702833336790505</v>
-      </c>
-      <c r="D202" s="0">
-        <v>-13.768200132822104</v>
+        <v>-13.672625961429164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>